<commit_message>
Updated code and removed error
</commit_message>
<xml_diff>
--- a/Carrick_AutomatedTest/Carrick_Automation/TestData/MaxDFRValidation.xlsx
+++ b/Carrick_AutomatedTest/Carrick_Automation/TestData/MaxDFRValidation.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64D96193-6430-4015-B840-A8184AA21D11}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7349551-8CFE-42C2-A100-7A19873B73C4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>DeviceName</t>
   </si>
@@ -52,9 +52,6 @@
     <t>10.75.58.51</t>
   </si>
   <si>
-    <t>500</t>
-  </si>
-  <si>
     <t>MaxDFR_Min</t>
   </si>
   <si>
@@ -62,6 +59,21 @@
   </si>
   <si>
     <t>MaxDFR_Max</t>
+  </si>
+  <si>
+    <t>PrefaultTime</t>
+  </si>
+  <si>
+    <t>1000</t>
+  </si>
+  <si>
+    <t>1200</t>
+  </si>
+  <si>
+    <t>31000</t>
+  </si>
+  <si>
+    <t>400</t>
   </si>
 </sst>
 </file>
@@ -383,7 +395,7 @@
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -401,63 +413,68 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="1" t="s">
         <v>9</v>
       </c>
       <c r="F2" s="1">
         <v>409026540</v>
       </c>
-      <c r="G2" s="1">
-        <v>400</v>
+      <c r="G2" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I2" s="1">
-        <v>31000</v>
-      </c>
-      <c r="J2" s="1"/>
+        <v>15</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">

</xml_diff>